<commit_message>
Added Credentials from Assts
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -171,98 +171,181 @@
     <t>StoreNumber.txt</t>
   </si>
   <si>
+    <t>API_OrderUpdate_RequestFormat</t>
+  </si>
+  <si>
+    <t>API_ClaimUpdate_RequestFormat</t>
+  </si>
+  <si>
+    <t>API_AppName</t>
+  </si>
+  <si>
+    <t>1128_API_AppName</t>
+  </si>
+  <si>
+    <t>API_OrderUpdate</t>
+  </si>
+  <si>
+    <t>API_ClaimUpdate</t>
+  </si>
+  <si>
+    <t>API_QA_EndPoint</t>
+  </si>
+  <si>
+    <t>API_PROD_EndPoint</t>
+  </si>
+  <si>
+    <t>1128_API_PROD_EndPoint</t>
+  </si>
+  <si>
+    <t>1128_API_OrderUpdate</t>
+  </si>
+  <si>
+    <t>1128_API_ClaimUpdate</t>
+  </si>
+  <si>
+    <t>1128_API_QA_EndPoint</t>
+  </si>
+  <si>
+    <t>API_OrderDownload</t>
+  </si>
+  <si>
+    <t>API_ClaimDownload</t>
+  </si>
+  <si>
+    <t>1128_API_OrderDownload</t>
+  </si>
+  <si>
+    <t>1128_API_ClaimDownload</t>
+  </si>
+  <si>
+    <t>Alert_URL</t>
+  </si>
+  <si>
+    <t>1128_Alert_URL</t>
+  </si>
+  <si>
+    <t>API_OrderDownload_RequestFormat</t>
+  </si>
+  <si>
+    <t>API_ClaimDownload_RequestFormat</t>
+  </si>
+  <si>
+    <t>API_Source</t>
+  </si>
+  <si>
+    <t>1128_API_Source</t>
+  </si>
+  <si>
+    <t>API_Version</t>
+  </si>
+  <si>
+    <t>1128_API_Version</t>
+  </si>
+  <si>
     <t>{
- "appName": "&lt;AppName&gt;",
+ "appName": "&lt;appName&gt;",
  "format": "json",
- "param{      
-        "decisionList": [
+ "param": {
+  "beginTime": "&lt;beginTime&gt;",
+  "endTime": "&lt;endTime&gt;"
+ },
+ "sign": "",
+ "source": "&lt;source&gt;",
+ "timestamp": "&lt;timestamp&gt;",
+ "version": "&lt;version&gt;"
+}</t>
+  </si>
+  <si>
+    <t>API_Download_LastNDays</t>
+  </si>
+  <si>
+    <t>1128_API_Download_LastNDays</t>
+  </si>
+  <si>
+    <t>{
+ "appName": "&lt;appName&gt;",
+ "format": "json",
+ "param": [{
+         "orderId": "&lt;orderId&gt;", "poNbr": "&lt;poNbr&gt;", "receiptNbr":  "&lt;receiptNbr&gt;","resultCode": "&lt;resultCode&gt;","resultMsg": "&lt;resultMsg&gt;"}],
+ "sign": "",
+ "source": "RPA",
+ "timestamp": "&lt;timestamp&gt;",
+ "version": "&lt;version&gt;"
+}</t>
+  </si>
+  <si>
+    <t>{
+ "appName": "&lt;appName&gt;",
+ "format": "json",
+ "param": [
          {
     "orderId": "&lt;orderId&gt;",
-          "poNbr":"&lt;poNbr&gt;",
-   "receiptNbr": "&lt;receiptNbr&gt;",
+          "afsId": "&lt;afsId&gt;",
+   "compensationId": "&lt;compensationId&gt;",
           "resultCode": "&lt;resultCode&gt;",
-          "resultMsg": "&lt;resultMsg&gt;",
-         }, 
+          "resultMsg": "&lt;resultMsg&gt;"
+         }
          ],
  "sign": "",
  "source": "RPA",
  "timestamp": "&lt;timestamp&gt;",
- "version": "1.0"
+ "version": "&lt;version&gt;"
 }</t>
   </si>
   <si>
-    <t>API_OrderUpdate_RequestFormat</t>
-  </si>
-  <si>
-    <t>API_ClaimUpdate_RequestFormat</t>
-  </si>
-  <si>
-    <t>{
- "appName": "&lt;AppName&gt;",
- "format": "json",
- "param{      
-        "compensationList": [
-         {
-    "orderId": "&lt;orderId&gt;",
-          "afsId": "&lt;afsId&gt;"
-   "compensationId": "&lt;compensationId&gt;",
-          "resultCode": "&lt;resultCode&gt;",
-          "resultMsg": "&lt;resultMsg&gt;",
-         }, 
-         ],
- "sign": "",
- "source": "RPA",
- "timestamp": "&lt;timestamp&gt;",
- "version": "1.0"
-}</t>
-  </si>
-  <si>
-    <t>API_AppName</t>
-  </si>
-  <si>
-    <t>1128_API_AppName</t>
-  </si>
-  <si>
-    <t>API_OrderUpdate</t>
-  </si>
-  <si>
-    <t>API_ClaimUpdate</t>
-  </si>
-  <si>
-    <t>API_QA_EndPoint</t>
-  </si>
-  <si>
-    <t>API_PROD_EndPoint</t>
-  </si>
-  <si>
-    <t>1128_API_PROD_EndPoint</t>
-  </si>
-  <si>
-    <t>1128_API_OrderUpdate</t>
-  </si>
-  <si>
-    <t>1128_API_ClaimUpdate</t>
-  </si>
-  <si>
-    <t>1128_API_QA_EndPoint</t>
-  </si>
-  <si>
-    <t>API_OrderDownload</t>
-  </si>
-  <si>
-    <t>API_ClaimDownload</t>
-  </si>
-  <si>
-    <t>1128_API_OrderDownload</t>
-  </si>
-  <si>
-    <t>1128_API_ClaimDownload</t>
-  </si>
-  <si>
-    <t>Alert_URL</t>
-  </si>
-  <si>
-    <t>1128_Alert_URL</t>
+    <t>BusinessException_MailReceiver</t>
+  </si>
+  <si>
+    <t>1128_BusinessException_MailReceiver</t>
+  </si>
+  <si>
+    <t>SystemException_MailReceiver</t>
+  </si>
+  <si>
+    <t>1128_SystemException_MailReceiver</t>
+  </si>
+  <si>
+    <t>Notification_MailReceiver</t>
+  </si>
+  <si>
+    <t>1128_Notification_MailReceiver</t>
+  </si>
+  <si>
+    <t>BusinessException_MailCopyTo</t>
+  </si>
+  <si>
+    <t>1128_BusinessException_MailCopyTo</t>
+  </si>
+  <si>
+    <t>SystemException_MailCopyTo</t>
+  </si>
+  <si>
+    <t>1128_SystemException_MailCopyTo</t>
+  </si>
+  <si>
+    <t>Notification_MailCopyTo</t>
+  </si>
+  <si>
+    <t>1128_Notification_MailCopyTo</t>
+  </si>
+  <si>
+    <t>Completed_MailSubject</t>
+  </si>
+  <si>
+    <t>Completed_MailBody</t>
+  </si>
+  <si>
+    <t>API_UpdateTimeOut_InSeconds</t>
+  </si>
+  <si>
+    <t>1128_API_UpdateTimeOut_InSeconds</t>
+  </si>
+  <si>
+    <t>API_DownloadTimeOut_InSeconds</t>
+  </si>
+  <si>
+    <t>1128_API_DownloadTimeOut_InSeconds</t>
   </si>
 </sst>
 </file>
@@ -309,7 +392,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,20 +750,36 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -689,10 +790,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,6 +990,16 @@
         <v>30</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -897,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="65.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,66 +1037,154 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
         <v>65</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified logic for order handling vendornumber checking into name checking
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -346,6 +346,84 @@
   </si>
   <si>
     <t>1128_API_DownloadTimeOut_InSeconds</t>
+  </si>
+  <si>
+    <t>订单-01-订单号错误</t>
+  </si>
+  <si>
+    <t>BE-Order-1</t>
+  </si>
+  <si>
+    <t>BE-Order-2</t>
+  </si>
+  <si>
+    <t>BE-Order-3</t>
+  </si>
+  <si>
+    <t>BE-Order-4</t>
+  </si>
+  <si>
+    <t>订单-02-非初次收货</t>
+  </si>
+  <si>
+    <t>订单-03-商品NOF</t>
+  </si>
+  <si>
+    <t>订单-04-收货数量大于订单</t>
+  </si>
+  <si>
+    <t>索赔-01-商品NOF</t>
+  </si>
+  <si>
+    <t>BE-Claim-4</t>
+  </si>
+  <si>
+    <t>BE-Claim-1</t>
+  </si>
+  <si>
+    <t>BE-Claim-2</t>
+  </si>
+  <si>
+    <t>BE-Claim-3</t>
+  </si>
+  <si>
+    <t>索赔-02-供应商号错误</t>
+  </si>
+  <si>
+    <t>索赔-04-索赔金额错误</t>
+  </si>
+  <si>
+    <t>1128_VendorNumbers</t>
+  </si>
+  <si>
+    <t>VendorNumbers</t>
+  </si>
+  <si>
+    <t>索赔-03-成本超100%/SMART当前实际索赔成本/&lt;SmartCost&gt;</t>
+  </si>
+  <si>
+    <t>1128_ClaimLowerLimit</t>
+  </si>
+  <si>
+    <t>1128_ClaimUpperLimit</t>
+  </si>
+  <si>
+    <t>ClaimLowerLimit</t>
+  </si>
+  <si>
+    <t>ClaimUpperLimit</t>
+  </si>
+  <si>
+    <t>订单-05-供应商号错误</t>
+  </si>
+  <si>
+    <t>BE-Order-5</t>
+  </si>
+  <si>
+    <t>VendorNames</t>
+  </si>
+  <si>
+    <t>1128_VendorNames</t>
   </si>
 </sst>
 </file>
@@ -790,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,6 +1078,78 @@
         <v>93</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1008,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="65.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,6 +1337,38 @@
         <v>97</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>